<commit_message>
sanity checks on linux
</commit_message>
<xml_diff>
--- a/source_data_files_ncomms/SourceDataFigure2B.xlsx
+++ b/source_data_files_ncomms/SourceDataFigure2B.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6997" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7431" uniqueCount="206">
   <si>
     <t>data_1</t>
   </si>
@@ -525,6 +525,54 @@
   </si>
   <si>
     <t>data_2</t>
+  </si>
+  <si>
+    <t>condlabels</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>cellId</t>
+  </si>
+  <si>
+    <t>data_1</t>
+  </si>
+  <si>
+    <t>data_2</t>
+  </si>
+  <si>
+    <t>data_3</t>
+  </si>
+  <si>
+    <t>data_4</t>
+  </si>
+  <si>
+    <t>condlabels</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>cellId</t>
+  </si>
+  <si>
+    <t>data_1</t>
+  </si>
+  <si>
+    <t>data_2</t>
+  </si>
+  <si>
+    <t>data_3</t>
+  </si>
+  <si>
+    <t>data_4</t>
   </si>
   <si>
     <t>condlabels</t>
@@ -605,7 +653,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -614,13 +662,17 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,22 +695,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2">
@@ -675,7 +727,7 @@
         <v>0.71698113207547176</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F2" s="0">
         <v>1</v>
@@ -695,7 +747,7 @@
         <v>0.97058823529411764</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F3" s="0">
         <v>2</v>
@@ -715,7 +767,7 @@
         <v>1.0283018867924529</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F4" s="0">
         <v>3</v>
@@ -735,7 +787,7 @@
         <v>0.45945945945945948</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F5" s="0">
         <v>4</v>
@@ -755,7 +807,7 @@
         <v>1.0499999999999998</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F6" s="0">
         <v>5</v>
@@ -775,7 +827,7 @@
         <v>0.61224489795918369</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F7" s="0">
         <v>6</v>
@@ -795,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F8" s="0">
         <v>7</v>
@@ -815,7 +867,7 @@
         <v>0.97777777777777763</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F9" s="0">
         <v>8</v>
@@ -835,7 +887,7 @@
         <v>0.5357142857142857</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F10" s="0">
         <v>9</v>
@@ -855,7 +907,7 @@
         <v>0.84615384615384603</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F11" s="0">
         <v>10</v>
@@ -875,7 +927,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F12" s="0">
         <v>11</v>
@@ -895,7 +947,7 @@
         <v>1.0860215053763442</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F13" s="0">
         <v>12</v>
@@ -915,7 +967,7 @@
         <v>0.97058823529411764</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F14" s="0">
         <v>13</v>
@@ -935,7 +987,7 @@
         <v>0.61818181818181817</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F15" s="0">
         <v>14</v>
@@ -955,7 +1007,7 @@
         <v>0.87499999999999989</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F16" s="0">
         <v>15</v>
@@ -975,7 +1027,7 @@
         <v>0.80487804878048785</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F17" s="0">
         <v>16</v>
@@ -995,7 +1047,7 @@
         <v>1.1818181818181819</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F18" s="0">
         <v>17</v>
@@ -1015,7 +1067,7 @@
         <v>0.83050847457627119</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F19" s="0">
         <v>18</v>
@@ -1035,7 +1087,7 @@
         <v>0.92105263157894723</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F20" s="0">
         <v>19</v>
@@ -1055,7 +1107,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F21" s="0">
         <v>20</v>
@@ -1075,7 +1127,7 @@
         <v>0.82828282828282829</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F22" s="0">
         <v>21</v>
@@ -1095,7 +1147,7 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F23" s="0">
         <v>22</v>
@@ -1115,7 +1167,7 @@
         <v>1.4102564102564099</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F24" s="0">
         <v>23</v>
@@ -1135,7 +1187,7 @@
         <v>0.70731707317073178</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F25" s="0">
         <v>24</v>
@@ -1155,7 +1207,7 @@
         <v>0.89743589743589725</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F26" s="0">
         <v>25</v>
@@ -1175,7 +1227,7 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F27" s="0">
         <v>26</v>
@@ -1195,7 +1247,7 @@
         <v>0.73913043478260854</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F28" s="0">
         <v>27</v>
@@ -1215,7 +1267,7 @@
         <v>0.59649122807017541</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F29" s="0">
         <v>28</v>
@@ -1235,7 +1287,7 @@
         <v>0.75</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F30" s="0">
         <v>29</v>
@@ -1255,7 +1307,7 @@
         <v>0.35802469135802473</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F31" s="0">
         <v>30</v>
@@ -1275,7 +1327,7 @@
         <v>0.69230769230769218</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F32" s="0">
         <v>31</v>
@@ -1295,7 +1347,7 @@
         <v>0.5116279069767441</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F33" s="0">
         <v>32</v>
@@ -1315,7 +1367,7 @@
         <v>0.28571428571428575</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F34" s="0">
         <v>33</v>
@@ -1335,7 +1387,7 @@
         <v>0.70491803278688536</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F35" s="0">
         <v>34</v>
@@ -1355,7 +1407,7 @@
         <v>0.67272727272727273</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F36" s="0">
         <v>35</v>
@@ -1375,7 +1427,7 @@
         <v>0.84057971014492749</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F37" s="0">
         <v>36</v>
@@ -1395,7 +1447,7 @@
         <v>1.1111111111111112</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F38" s="0">
         <v>37</v>
@@ -1415,7 +1467,7 @@
         <v>0.7272727272727274</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F39" s="0">
         <v>38</v>
@@ -1435,7 +1487,7 @@
         <v>0.85714285714285732</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F40" s="0">
         <v>39</v>
@@ -1455,7 +1507,7 @@
         <v>0.94736842105263153</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F41" s="0">
         <v>40</v>
@@ -1475,7 +1527,7 @@
         <v>0.75555555555555554</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F42" s="0">
         <v>41</v>
@@ -1495,7 +1547,7 @@
         <v>0.90196078431372551</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F43" s="0">
         <v>42</v>
@@ -1515,7 +1567,7 @@
         <v>0.87804878048780488</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F44" s="0">
         <v>43</v>
@@ -1535,7 +1587,7 @@
         <v>0.95833333333333326</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F45" s="0">
         <v>44</v>
@@ -1555,7 +1607,7 @@
         <v>1.0144927536231882</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F46" s="0">
         <v>45</v>
@@ -1575,7 +1627,7 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F47" s="0">
         <v>46</v>
@@ -1595,7 +1647,7 @@
         <v>0.76344086021505375</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F48" s="0">
         <v>47</v>
@@ -1615,7 +1667,7 @@
         <v>0.64000000000000001</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F49" s="0">
         <v>48</v>
@@ -1635,7 +1687,7 @@
         <v>0.85294117647058831</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F50" s="0">
         <v>49</v>
@@ -1655,7 +1707,7 @@
         <v>1.0537634408602152</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F51" s="0">
         <v>50</v>
@@ -1675,7 +1727,7 @@
         <v>0.84615384615384615</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F52" s="0">
         <v>51</v>
@@ -1695,7 +1747,7 @@
         <v>0.5</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F53" s="0">
         <v>52</v>
@@ -1715,7 +1767,7 @@
         <v>0.91836734693877553</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F54" s="0">
         <v>53</v>
@@ -1735,7 +1787,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F55" s="0">
         <v>54</v>
@@ -1755,7 +1807,7 @@
         <v>0.58974358974358965</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F56" s="0">
         <v>55</v>
@@ -1775,7 +1827,7 @@
         <v>0.69565217391304357</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F57" s="0">
         <v>56</v>
@@ -1795,7 +1847,7 @@
         <v>0.76086956521739124</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F58" s="0">
         <v>57</v>
@@ -1815,7 +1867,7 @@
         <v>0.77192982456140347</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F59" s="0">
         <v>58</v>
@@ -1835,7 +1887,7 @@
         <v>0.8717948717948717</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F60" s="0">
         <v>59</v>
@@ -1855,7 +1907,7 @@
         <v>0.91891891891891897</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F61" s="0">
         <v>60</v>
@@ -1875,7 +1927,7 @@
         <v>1.0677966101694916</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F62" s="0">
         <v>61</v>
@@ -1895,7 +1947,7 @@
         <v>0.9375</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F63" s="0">
         <v>62</v>
@@ -1915,7 +1967,7 @@
         <v>1.0322580645161292</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F64" s="0">
         <v>63</v>
@@ -1935,7 +1987,7 @@
         <v>0.69999999999999996</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F65" s="0">
         <v>64</v>
@@ -1955,7 +2007,7 @@
         <v>0.80000000000000016</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F66" s="0">
         <v>65</v>
@@ -1975,7 +2027,7 @@
         <v>1.0384615384615385</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F67" s="0">
         <v>66</v>
@@ -1995,7 +2047,7 @@
         <v>0.60344827586206884</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F68" s="0">
         <v>67</v>
@@ -2015,7 +2067,7 @@
         <v>0.72340425531914887</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F69" s="0">
         <v>68</v>
@@ -2035,7 +2087,7 @@
         <v>0.70370370370370372</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F70" s="0">
         <v>69</v>
@@ -2055,7 +2107,7 @@
         <v>0.98571428571428588</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F71" s="0">
         <v>70</v>
@@ -2075,7 +2127,7 @@
         <v>0.90909090909090917</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F72" s="0">
         <v>71</v>
@@ -2095,7 +2147,7 @@
         <v>0.97435897435897423</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F73" s="0">
         <v>72</v>
@@ -2115,7 +2167,7 @@
         <v>0.62096774193548387</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F74" s="0">
         <v>73</v>
@@ -2135,7 +2187,7 @@
         <v>1.0263157894736843</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F75" s="0">
         <v>74</v>
@@ -2155,7 +2207,7 @@
         <v>0.71999999999999997</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F76" s="0">
         <v>75</v>
@@ -2175,7 +2227,7 @@
         <v>0.57377049180327866</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F77" s="0">
         <v>76</v>
@@ -2195,7 +2247,7 @@
         <v>0.88571428571428579</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F78" s="0">
         <v>77</v>
@@ -2215,7 +2267,7 @@
         <v>0.15702479338842978</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F79" s="0">
         <v>78</v>
@@ -2235,7 +2287,7 @@
         <v>0.55882352941176472</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F80" s="0">
         <v>79</v>
@@ -2255,7 +2307,7 @@
         <v>0.83333333333333348</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F81" s="0">
         <v>80</v>
@@ -2275,7 +2327,7 @@
         <v>0.91869918699186992</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F82" s="0">
         <v>81</v>
@@ -2295,7 +2347,7 @@
         <v>1.1272727272727272</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F83" s="0">
         <v>82</v>
@@ -2315,7 +2367,7 @@
         <v>0.64864864864864868</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F84" s="0">
         <v>83</v>
@@ -2335,7 +2387,7 @@
         <v>0.78082191780821919</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F85" s="0">
         <v>84</v>
@@ -2355,7 +2407,7 @@
         <v>0.59740259740259738</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F86" s="0">
         <v>85</v>
@@ -2375,7 +2427,7 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F87" s="0">
         <v>86</v>
@@ -2395,7 +2447,7 @@
         <v>0.67741935483870963</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F88" s="0">
         <v>87</v>
@@ -2415,7 +2467,7 @@
         <v>1.0789473684210527</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="F89" s="0">
         <v>88</v>
@@ -2435,7 +2487,7 @@
         <v>0.71698113207547176</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F90" s="0">
         <v>1</v>
@@ -2455,7 +2507,7 @@
         <v>1.088235294117647</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F91" s="0">
         <v>2</v>
@@ -2475,7 +2527,7 @@
         <v>1.0094339622641511</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F92" s="0">
         <v>3</v>
@@ -2495,7 +2547,7 @@
         <v>0.67567567567567577</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F93" s="0">
         <v>4</v>
@@ -2515,7 +2567,7 @@
         <v>0.40000000000000002</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F94" s="0">
         <v>5</v>
@@ -2535,7 +2587,7 @@
         <v>0.79591836734693888</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F95" s="0">
         <v>6</v>
@@ -2555,7 +2607,7 @@
         <v>0.55384615384615388</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F96" s="0">
         <v>7</v>
@@ -2575,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F97" s="0">
         <v>8</v>
@@ -2595,7 +2647,7 @@
         <v>0.92857142857142849</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F98" s="0">
         <v>9</v>
@@ -2615,7 +2667,7 @@
         <v>0.90384615384615385</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F99" s="0">
         <v>10</v>
@@ -2635,7 +2687,7 @@
         <v>1.0937499999999998</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F100" s="0">
         <v>11</v>
@@ -2655,7 +2707,7 @@
         <v>0.77419354838709686</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F101" s="0">
         <v>12</v>
@@ -2675,7 +2727,7 @@
         <v>0.94117647058823539</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F102" s="0">
         <v>13</v>
@@ -2695,7 +2747,7 @@
         <v>0.89090909090909098</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F103" s="0">
         <v>14</v>
@@ -2715,7 +2767,7 @@
         <v>1.2916666666666667</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F104" s="0">
         <v>15</v>
@@ -2735,7 +2787,7 @@
         <v>1</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F105" s="0">
         <v>16</v>
@@ -2755,7 +2807,7 @@
         <v>1.1818181818181819</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F106" s="0">
         <v>17</v>
@@ -2775,7 +2827,7 @@
         <v>0.6271186440677966</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F107" s="0">
         <v>18</v>
@@ -2795,7 +2847,7 @@
         <v>0.6578947368421052</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F108" s="0">
         <v>19</v>
@@ -2815,7 +2867,7 @@
         <v>0.66666666666666674</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F109" s="0">
         <v>20</v>
@@ -2835,7 +2887,7 @@
         <v>0.65656565656565646</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F110" s="0">
         <v>21</v>
@@ -2855,7 +2907,7 @@
         <v>0.67708333333333326</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F111" s="0">
         <v>22</v>
@@ -2875,7 +2927,7 @@
         <v>0.8717948717948717</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F112" s="0">
         <v>23</v>
@@ -2895,7 +2947,7 @@
         <v>0.95121951219512213</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F113" s="0">
         <v>24</v>
@@ -2915,7 +2967,7 @@
         <v>0.79487179487179471</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F114" s="0">
         <v>25</v>
@@ -2935,7 +2987,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F115" s="0">
         <v>26</v>
@@ -2955,7 +3007,7 @@
         <v>0.85507246376811585</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F116" s="0">
         <v>27</v>
@@ -2975,7 +3027,7 @@
         <v>0.70175438596491235</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F117" s="0">
         <v>28</v>
@@ -2995,7 +3047,7 @@
         <v>0.92499999999999982</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F118" s="0">
         <v>29</v>
@@ -3015,7 +3067,7 @@
         <v>0.44444444444444442</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F119" s="0">
         <v>30</v>
@@ -3035,7 +3087,7 @@
         <v>0.61538461538461531</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F120" s="0">
         <v>31</v>
@@ -3055,7 +3107,7 @@
         <v>0.60465116279069764</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F121" s="0">
         <v>32</v>
@@ -3075,7 +3127,7 @@
         <v>0.3714285714285715</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F122" s="0">
         <v>33</v>
@@ -3095,7 +3147,7 @@
         <v>0.83606557377049184</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F123" s="0">
         <v>34</v>
@@ -3115,7 +3167,7 @@
         <v>0.54545454545454553</v>
       </c>
       <c r="E124" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F124" s="0">
         <v>35</v>
@@ -3135,7 +3187,7 @@
         <v>0.81159420289855067</v>
       </c>
       <c r="E125" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F125" s="0">
         <v>36</v>
@@ -3155,7 +3207,7 @@
         <v>0.88888888888888895</v>
       </c>
       <c r="E126" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F126" s="0">
         <v>37</v>
@@ -3175,7 +3227,7 @@
         <v>1.0454545454545454</v>
       </c>
       <c r="E127" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F127" s="0">
         <v>38</v>
@@ -3195,7 +3247,7 @@
         <v>0.77142857142857157</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F128" s="0">
         <v>39</v>
@@ -3215,7 +3267,7 @@
         <v>1.263157894736842</v>
       </c>
       <c r="E129" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F129" s="0">
         <v>40</v>
@@ -3235,7 +3287,7 @@
         <v>0.88888888888888895</v>
       </c>
       <c r="E130" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F130" s="0">
         <v>41</v>
@@ -3255,7 +3307,7 @@
         <v>0.81372549019607843</v>
       </c>
       <c r="E131" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F131" s="0">
         <v>42</v>
@@ -3275,7 +3327,7 @@
         <v>0.97560975609756106</v>
       </c>
       <c r="E132" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F132" s="0">
         <v>43</v>
@@ -3295,7 +3347,7 @@
         <v>0.75</v>
       </c>
       <c r="E133" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F133" s="0">
         <v>44</v>
@@ -3315,7 +3367,7 @@
         <v>0.73913043478260854</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F134" s="0">
         <v>45</v>
@@ -3335,7 +3387,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E135" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F135" s="0">
         <v>46</v>
@@ -3355,7 +3407,7 @@
         <v>0.82795698924731187</v>
       </c>
       <c r="E136" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F136" s="0">
         <v>47</v>
@@ -3375,7 +3427,7 @@
         <v>1.1600000000000001</v>
       </c>
       <c r="E137" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F137" s="0">
         <v>48</v>
@@ -3395,7 +3447,7 @@
         <v>0.91176470588235292</v>
       </c>
       <c r="E138" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F138" s="0">
         <v>49</v>
@@ -3415,7 +3467,7 @@
         <v>0.90322580645161288</v>
       </c>
       <c r="E139" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F139" s="0">
         <v>50</v>
@@ -3435,7 +3487,7 @@
         <v>0.44615384615384623</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F140" s="0">
         <v>51</v>
@@ -3455,7 +3507,7 @@
         <v>0.57142857142857151</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F141" s="0">
         <v>52</v>
@@ -3475,7 +3527,7 @@
         <v>0.85714285714285698</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F142" s="0">
         <v>53</v>
@@ -3495,7 +3547,7 @@
         <v>0.7142857142857143</v>
       </c>
       <c r="E143" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F143" s="0">
         <v>54</v>
@@ -3515,7 +3567,7 @@
         <v>0.79487179487179471</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F144" s="0">
         <v>55</v>
@@ -3535,7 +3587,7 @@
         <v>0.78260869565217395</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F145" s="0">
         <v>56</v>
@@ -3555,7 +3607,7 @@
         <v>0.65217391304347838</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F146" s="0">
         <v>57</v>
@@ -3575,7 +3627,7 @@
         <v>0.84210526315789469</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F147" s="0">
         <v>58</v>
@@ -3595,7 +3647,7 @@
         <v>0.97435897435897423</v>
       </c>
       <c r="E148" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F148" s="0">
         <v>59</v>
@@ -3615,7 +3667,7 @@
         <v>1.2432432432432432</v>
       </c>
       <c r="E149" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F149" s="0">
         <v>60</v>
@@ -3635,7 +3687,7 @@
         <v>0.40677966101694912</v>
       </c>
       <c r="E150" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F150" s="0">
         <v>61</v>
@@ -3655,7 +3707,7 @@
         <v>0.81249999999999989</v>
       </c>
       <c r="E151" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F151" s="0">
         <v>62</v>
@@ -3675,7 +3727,7 @@
         <v>0.61290322580645162</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F152" s="0">
         <v>63</v>
@@ -3695,7 +3747,7 @@
         <v>0.59999999999999998</v>
       </c>
       <c r="E153" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F153" s="0">
         <v>64</v>
@@ -3715,7 +3767,7 @@
         <v>1.0571428571428572</v>
       </c>
       <c r="E154" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F154" s="0">
         <v>65</v>
@@ -3735,7 +3787,7 @@
         <v>1.0384615384615385</v>
       </c>
       <c r="E155" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F155" s="0">
         <v>66</v>
@@ -3755,7 +3807,7 @@
         <v>0.79310344827586199</v>
       </c>
       <c r="E156" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F156" s="0">
         <v>67</v>
@@ -3775,7 +3827,7 @@
         <v>0.8085106382978724</v>
       </c>
       <c r="E157" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F157" s="0">
         <v>68</v>
@@ -3795,7 +3847,7 @@
         <v>0.46296296296296297</v>
       </c>
       <c r="E158" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F158" s="0">
         <v>69</v>
@@ -3815,7 +3867,7 @@
         <v>0.9571428571428573</v>
       </c>
       <c r="E159" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F159" s="0">
         <v>70</v>
@@ -3835,7 +3887,7 @@
         <v>0.79545454545454541</v>
       </c>
       <c r="E160" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F160" s="0">
         <v>71</v>
@@ -3855,7 +3907,7 @@
         <v>0.64102564102564097</v>
       </c>
       <c r="E161" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F161" s="0">
         <v>72</v>
@@ -3875,7 +3927,7 @@
         <v>0.68548387096774199</v>
       </c>
       <c r="E162" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F162" s="0">
         <v>73</v>
@@ -3895,7 +3947,7 @@
         <v>0.78947368421052633</v>
       </c>
       <c r="E163" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F163" s="0">
         <v>74</v>
@@ -3915,7 +3967,7 @@
         <v>0.58000000000000007</v>
       </c>
       <c r="E164" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F164" s="0">
         <v>75</v>
@@ -3935,7 +3987,7 @@
         <v>0.44262295081967218</v>
       </c>
       <c r="E165" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F165" s="0">
         <v>76</v>
@@ -3955,7 +4007,7 @@
         <v>0.65714285714285714</v>
       </c>
       <c r="E166" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F166" s="0">
         <v>77</v>
@@ -3975,7 +4027,7 @@
         <v>0.54545454545454553</v>
       </c>
       <c r="E167" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F167" s="0">
         <v>78</v>
@@ -3995,7 +4047,7 @@
         <v>0.97058823529411764</v>
       </c>
       <c r="E168" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F168" s="0">
         <v>79</v>
@@ -4015,7 +4067,7 @@
         <v>0.83333333333333348</v>
       </c>
       <c r="E169" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F169" s="0">
         <v>80</v>
@@ -4035,7 +4087,7 @@
         <v>1.065040650406504</v>
       </c>
       <c r="E170" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F170" s="0">
         <v>81</v>
@@ -4055,7 +4107,7 @@
         <v>1.0727272727272728</v>
       </c>
       <c r="E171" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F171" s="0">
         <v>82</v>
@@ -4075,7 +4127,7 @@
         <v>0.54054054054054057</v>
       </c>
       <c r="E172" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F172" s="0">
         <v>83</v>
@@ -4095,7 +4147,7 @@
         <v>0.80821917808219179</v>
       </c>
       <c r="E173" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F173" s="0">
         <v>84</v>
@@ -4115,7 +4167,7 @@
         <v>0.74025974025974028</v>
       </c>
       <c r="E174" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F174" s="0">
         <v>85</v>
@@ -4135,7 +4187,7 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="E175" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F175" s="0">
         <v>86</v>
@@ -4155,7 +4207,7 @@
         <v>0.90322580645161299</v>
       </c>
       <c r="E176" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F176" s="0">
         <v>87</v>
@@ -4175,7 +4227,7 @@
         <v>1.0526315789473684</v>
       </c>
       <c r="E177" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F177" s="0">
         <v>88</v>
@@ -6734,22 +6786,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2">
@@ -6766,7 +6818,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F2" s="0">
         <v>1</v>
@@ -6786,7 +6838,7 @@
         <v>0.70512820512820495</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F3" s="0">
         <v>2</v>
@@ -6806,7 +6858,7 @@
         <v>0.82812499999999989</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F4" s="0">
         <v>3</v>
@@ -6826,7 +6878,7 @@
         <v>0.8717948717948717</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F5" s="0">
         <v>4</v>
@@ -6846,7 +6898,7 @@
         <v>0.60869565217391308</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F6" s="0">
         <v>5</v>
@@ -6866,7 +6918,7 @@
         <v>0.76086956521739124</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F7" s="0">
         <v>6</v>
@@ -6886,7 +6938,7 @@
         <v>0.67346938775510201</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F8" s="0">
         <v>7</v>
@@ -6906,7 +6958,7 @@
         <v>0.5178571428571429</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F9" s="0">
         <v>8</v>
@@ -6926,7 +6978,7 @@
         <v>0.74285714285714299</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F10" s="0">
         <v>9</v>
@@ -6946,7 +6998,7 @@
         <v>0.18367346938775508</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F11" s="0">
         <v>10</v>
@@ -6966,7 +7018,7 @@
         <v>0.95683453237410077</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F12" s="0">
         <v>11</v>
@@ -6986,7 +7038,7 @@
         <v>0.73134328358208955</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F13" s="0">
         <v>12</v>
@@ -7006,7 +7058,7 @@
         <v>0.85526315789473673</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F14" s="0">
         <v>13</v>
@@ -7026,7 +7078,7 @@
         <v>0.58510638297872331</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F15" s="0">
         <v>14</v>
@@ -7046,7 +7098,7 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F16" s="0">
         <v>15</v>
@@ -7066,7 +7118,7 @@
         <v>0.46875</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F17" s="0">
         <v>16</v>
@@ -7086,7 +7138,7 @@
         <v>0.85365853658536583</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F18" s="0">
         <v>17</v>
@@ -7106,7 +7158,7 @@
         <v>0.7272727272727274</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F19" s="0">
         <v>18</v>
@@ -7126,7 +7178,7 @@
         <v>0.72058823529411764</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F20" s="0">
         <v>19</v>
@@ -7146,7 +7198,7 @@
         <v>1.482758620689655</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F21" s="0">
         <v>20</v>
@@ -7166,7 +7218,7 @@
         <v>0.49122807017543862</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F22" s="0">
         <v>21</v>
@@ -7186,7 +7238,7 @@
         <v>0.51000000000000001</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F23" s="0">
         <v>22</v>
@@ -7206,7 +7258,7 @@
         <v>0.90196078431372551</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F24" s="0">
         <v>23</v>
@@ -7226,7 +7278,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F25" s="0">
         <v>24</v>
@@ -7246,7 +7298,7 @@
         <v>0.875</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F26" s="0">
         <v>25</v>
@@ -7266,7 +7318,7 @@
         <v>0.63043478260869568</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F27" s="0">
         <v>26</v>
@@ -7286,7 +7338,7 @@
         <v>0.73333333333333328</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F28" s="0">
         <v>27</v>
@@ -7306,7 +7358,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F29" s="0">
         <v>28</v>
@@ -7326,7 +7378,7 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F30" s="0">
         <v>29</v>
@@ -7346,7 +7398,7 @@
         <v>0.70270270270270274</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F31" s="0">
         <v>30</v>
@@ -7366,7 +7418,7 @@
         <v>0.44262295081967218</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F32" s="0">
         <v>31</v>
@@ -7386,7 +7438,7 @@
         <v>0.99107142857142849</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F33" s="0">
         <v>32</v>
@@ -7406,7 +7458,7 @@
         <v>0.7450980392156864</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F34" s="0">
         <v>33</v>
@@ -7426,7 +7478,7 @@
         <v>0.85294117647058831</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F35" s="0">
         <v>34</v>
@@ -7446,7 +7498,7 @@
         <v>0.84374999999999989</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F36" s="0">
         <v>35</v>
@@ -7466,7 +7518,7 @@
         <v>0.67391304347826086</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F37" s="0">
         <v>36</v>
@@ -7486,7 +7538,7 @@
         <v>0.87999999999999989</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F38" s="0">
         <v>37</v>
@@ -7506,7 +7558,7 @@
         <v>0.87096774193548399</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F39" s="0">
         <v>38</v>
@@ -7526,7 +7578,7 @@
         <v>0.64102564102564097</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F40" s="0">
         <v>39</v>
@@ -7546,7 +7598,7 @@
         <v>0.88805970149253732</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F41" s="0">
         <v>40</v>
@@ -7566,7 +7618,7 @@
         <v>0.86259541984732835</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F42" s="0">
         <v>41</v>
@@ -7586,7 +7638,7 @@
         <v>0.94262295081967218</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F43" s="0">
         <v>42</v>
@@ -7606,7 +7658,7 @@
         <v>1.1388888888888888</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F44" s="0">
         <v>43</v>
@@ -7626,7 +7678,7 @@
         <v>0.92771084337349408</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F45" s="0">
         <v>44</v>
@@ -7646,7 +7698,7 @@
         <v>0.87654320987654311</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F46" s="0">
         <v>45</v>
@@ -7666,7 +7718,7 @@
         <v>0.68421052631578938</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F47" s="0">
         <v>46</v>
@@ -7686,7 +7738,7 @@
         <v>0.93506493506493504</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F48" s="0">
         <v>47</v>
@@ -7706,7 +7758,7 @@
         <v>0.42857142857142849</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F49" s="0">
         <v>48</v>
@@ -7726,7 +7778,7 @@
         <v>0.98000000000000009</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F50" s="0">
         <v>49</v>
@@ -7746,7 +7798,7 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F51" s="0">
         <v>50</v>
@@ -7766,7 +7818,7 @@
         <v>0.94000000000000006</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F52" s="0">
         <v>51</v>
@@ -7786,7 +7838,7 @@
         <v>0.91366906474820153</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F53" s="0">
         <v>52</v>
@@ -7806,7 +7858,7 @@
         <v>0.77551020408163263</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F54" s="0">
         <v>53</v>
@@ -7826,7 +7878,7 @@
         <v>0.45945945945945948</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F55" s="0">
         <v>54</v>
@@ -7846,7 +7898,7 @@
         <v>1.0833333333333333</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F56" s="0">
         <v>55</v>
@@ -7866,7 +7918,7 @@
         <v>0.96634615384615385</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F57" s="0">
         <v>56</v>
@@ -7886,7 +7938,7 @@
         <v>0.45454545454545459</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F58" s="0">
         <v>57</v>
@@ -7906,7 +7958,7 @@
         <v>0.90476190476190488</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F59" s="0">
         <v>58</v>
@@ -7926,7 +7978,7 @@
         <v>0.60638297872340419</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F60" s="0">
         <v>59</v>
@@ -7946,7 +7998,7 @@
         <v>1.0967741935483872</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F61" s="0">
         <v>60</v>
@@ -7966,7 +8018,7 @@
         <v>0.86111111111111105</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F62" s="0">
         <v>61</v>
@@ -7986,7 +8038,7 @@
         <v>0.72340425531914887</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F63" s="0">
         <v>62</v>
@@ -8006,7 +8058,7 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F64" s="0">
         <v>63</v>
@@ -8026,7 +8078,7 @@
         <v>0.87951807228915668</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F65" s="0">
         <v>64</v>
@@ -8046,7 +8098,7 @@
         <v>0.89705882352941169</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F66" s="0">
         <v>65</v>
@@ -8066,7 +8118,7 @@
         <v>0.52380952380952384</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F67" s="0">
         <v>66</v>
@@ -8086,7 +8138,7 @@
         <v>1.0555555555555556</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F68" s="0">
         <v>67</v>
@@ -8106,7 +8158,7 @@
         <v>1.2580645161290325</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F69" s="0">
         <v>68</v>
@@ -8126,7 +8178,7 @@
         <v>0.23622047244094491</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F70" s="0">
         <v>69</v>
@@ -8146,7 +8198,7 @@
         <v>0.83333333333333326</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F71" s="0">
         <v>70</v>
@@ -8166,7 +8218,7 @@
         <v>0.679245283018868</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F72" s="0">
         <v>71</v>
@@ -8186,7 +8238,7 @@
         <v>0.70769230769230773</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F73" s="0">
         <v>72</v>
@@ -8206,7 +8258,7 @@
         <v>0.71962616822429903</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F74" s="0">
         <v>73</v>
@@ -8226,7 +8278,7 @@
         <v>0.47540983606557385</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F75" s="0">
         <v>74</v>
@@ -8246,7 +8298,7 @@
         <v>0.6428571428571429</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F76" s="0">
         <v>75</v>
@@ -8266,7 +8318,7 @@
         <v>0.47619047619047628</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F77" s="0">
         <v>76</v>
@@ -8286,7 +8338,7 @@
         <v>0.57499999999999996</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F78" s="0">
         <v>77</v>
@@ -8306,7 +8358,7 @@
         <v>0.76923076923076916</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F79" s="0">
         <v>78</v>
@@ -8326,7 +8378,7 @@
         <v>0.31914893617021278</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F80" s="0">
         <v>79</v>
@@ -8346,7 +8398,7 @@
         <v>0.56164383561643838</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F81" s="0">
         <v>80</v>
@@ -8366,7 +8418,7 @@
         <v>0.48148148148148145</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F82" s="0">
         <v>81</v>
@@ -8386,7 +8438,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F83" s="0">
         <v>82</v>
@@ -8406,7 +8458,7 @@
         <v>1.0952380952380953</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F84" s="0">
         <v>83</v>
@@ -8426,7 +8478,7 @@
         <v>0.54098360655737709</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F85" s="0">
         <v>84</v>
@@ -8446,7 +8498,7 @@
         <v>0.80104712041884818</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F86" s="0">
         <v>85</v>
@@ -8466,7 +8518,7 @@
         <v>0.82978723404255328</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F87" s="0">
         <v>86</v>
@@ -8486,7 +8538,7 @@
         <v>0.41818181818181815</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F88" s="0">
         <v>87</v>
@@ -8506,7 +8558,7 @@
         <v>0.4285714285714286</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F89" s="0">
         <v>88</v>
@@ -8526,7 +8578,7 @@
         <v>0.5</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F90" s="0">
         <v>89</v>
@@ -8546,7 +8598,7 @@
         <v>0.59090909090909094</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F91" s="0">
         <v>90</v>
@@ -8566,7 +8618,7 @@
         <v>0.68674698795180722</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F92" s="0">
         <v>91</v>
@@ -8586,7 +8638,7 @@
         <v>0.79452054794520555</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F93" s="0">
         <v>92</v>
@@ -8606,7 +8658,7 @@
         <v>0.62195121951219512</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F94" s="0">
         <v>93</v>
@@ -8626,7 +8678,7 @@
         <v>0.78846153846153844</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F95" s="0">
         <v>94</v>
@@ -8646,7 +8698,7 @@
         <v>0.68421052631578938</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F96" s="0">
         <v>95</v>
@@ -8666,7 +8718,7 @@
         <v>0.53968253968253965</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F97" s="0">
         <v>96</v>
@@ -8686,7 +8738,7 @@
         <v>0.47499999999999998</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F98" s="0">
         <v>97</v>
@@ -8706,7 +8758,7 @@
         <v>0.54545454545454553</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F99" s="0">
         <v>98</v>
@@ -8726,7 +8778,7 @@
         <v>1.0322580645161292</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F100" s="0">
         <v>99</v>
@@ -8746,7 +8798,7 @@
         <v>1</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F101" s="0">
         <v>100</v>
@@ -8766,7 +8818,7 @@
         <v>1.0555555555555556</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F102" s="0">
         <v>101</v>
@@ -8786,7 +8838,7 @@
         <v>1.08955223880597</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F103" s="0">
         <v>102</v>
@@ -8806,7 +8858,7 @@
         <v>0.73170731707317083</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F104" s="0">
         <v>103</v>
@@ -8826,7 +8878,7 @@
         <v>0.87999999999999989</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F105" s="0">
         <v>104</v>
@@ -8846,7 +8898,7 @@
         <v>0.65384615384615374</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F106" s="0">
         <v>105</v>
@@ -8866,7 +8918,7 @@
         <v>0.75</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F107" s="0">
         <v>106</v>
@@ -8886,7 +8938,7 @@
         <v>0.78260869565217395</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F108" s="0">
         <v>107</v>
@@ -8906,7 +8958,7 @@
         <v>0.75</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F109" s="0">
         <v>108</v>
@@ -8926,7 +8978,7 @@
         <v>0.81034482758620685</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F110" s="0">
         <v>109</v>
@@ -8946,7 +8998,7 @@
         <v>0.86538461538461542</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F111" s="0">
         <v>110</v>
@@ -8966,7 +9018,7 @@
         <v>0.79245283018867918</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F112" s="0">
         <v>111</v>
@@ -8986,7 +9038,7 @@
         <v>0.68354430379746844</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F113" s="0">
         <v>112</v>
@@ -9006,7 +9058,7 @@
         <v>0.72222222222222232</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F114" s="0">
         <v>113</v>
@@ -9026,7 +9078,7 @@
         <v>0.47619047619047628</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F115" s="0">
         <v>114</v>
@@ -9046,7 +9098,7 @@
         <v>1.0222222222222221</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F116" s="0">
         <v>115</v>
@@ -9066,7 +9118,7 @@
         <v>0.7661290322580645</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F117" s="0">
         <v>116</v>
@@ -9086,7 +9138,7 @@
         <v>0.73239436619718312</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F118" s="0">
         <v>117</v>
@@ -9106,7 +9158,7 @@
         <v>0.74242424242424243</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F119" s="0">
         <v>118</v>
@@ -9126,7 +9178,7 @@
         <v>0.97777777777777763</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F120" s="0">
         <v>119</v>
@@ -9146,7 +9198,7 @@
         <v>0.53012048192771088</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F121" s="0">
         <v>120</v>
@@ -9166,7 +9218,7 @@
         <v>0.72499999999999998</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F122" s="0">
         <v>121</v>
@@ -9186,7 +9238,7 @@
         <v>0.65000000000000002</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F123" s="0">
         <v>122</v>
@@ -9206,7 +9258,7 @@
         <v>0.68749999999999989</v>
       </c>
       <c r="E124" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F124" s="0">
         <v>123</v>
@@ -9226,7 +9278,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E125" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F125" s="0">
         <v>1</v>
@@ -9246,7 +9298,7 @@
         <v>0.79487179487179471</v>
       </c>
       <c r="E126" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F126" s="0">
         <v>2</v>
@@ -9266,7 +9318,7 @@
         <v>0.81249999999999989</v>
       </c>
       <c r="E127" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F127" s="0">
         <v>3</v>
@@ -9286,7 +9338,7 @@
         <v>0.79487179487179471</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F128" s="0">
         <v>4</v>
@@ -9306,7 +9358,7 @@
         <v>0.52173913043478259</v>
       </c>
       <c r="E129" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F129" s="0">
         <v>5</v>
@@ -9326,7 +9378,7 @@
         <v>0.73913043478260876</v>
       </c>
       <c r="E130" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F130" s="0">
         <v>6</v>
@@ -9346,7 +9398,7 @@
         <v>0.77551020408163263</v>
       </c>
       <c r="E131" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F131" s="0">
         <v>7</v>
@@ -9366,7 +9418,7 @@
         <v>0.48214285714285715</v>
       </c>
       <c r="E132" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F132" s="0">
         <v>8</v>
@@ -9386,7 +9438,7 @@
         <v>0.94285714285714295</v>
       </c>
       <c r="E133" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F133" s="0">
         <v>9</v>
@@ -9406,7 +9458,7 @@
         <v>0.40816326530612246</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F134" s="0">
         <v>10</v>
@@ -9426,7 +9478,7 @@
         <v>0.90647482014388503</v>
       </c>
       <c r="E135" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F135" s="0">
         <v>11</v>
@@ -9446,7 +9498,7 @@
         <v>0.01492537313432836</v>
       </c>
       <c r="E136" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F136" s="0">
         <v>12</v>
@@ -9466,7 +9518,7 @@
         <v>0.8157894736842104</v>
       </c>
       <c r="E137" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F137" s="0">
         <v>13</v>
@@ -9486,7 +9538,7 @@
         <v>0.8085106382978724</v>
       </c>
       <c r="E138" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F138" s="0">
         <v>14</v>
@@ -9506,7 +9558,7 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="E139" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F139" s="0">
         <v>15</v>
@@ -9526,7 +9578,7 @@
         <v>0.59375</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F140" s="0">
         <v>16</v>
@@ -9546,7 +9598,7 @@
         <v>0.9390243902439025</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F141" s="0">
         <v>17</v>
@@ -9566,7 +9618,7 @@
         <v>0.63636363636363646</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F142" s="0">
         <v>18</v>
@@ -9586,7 +9638,7 @@
         <v>0.77941176470588236</v>
       </c>
       <c r="E143" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F143" s="0">
         <v>19</v>
@@ -9606,7 +9658,7 @@
         <v>0.72413793103448265</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F144" s="0">
         <v>20</v>
@@ -9626,7 +9678,7 @@
         <v>0.85964912280701766</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F145" s="0">
         <v>21</v>
@@ -9646,7 +9698,7 @@
         <v>0.70999999999999996</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F146" s="0">
         <v>22</v>
@@ -9666,7 +9718,7 @@
         <v>0.6470588235294118</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F147" s="0">
         <v>23</v>
@@ -9686,7 +9738,7 @@
         <v>0.68181818181818188</v>
       </c>
       <c r="E148" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F148" s="0">
         <v>24</v>
@@ -9706,7 +9758,7 @@
         <v>0.625</v>
       </c>
       <c r="E149" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F149" s="0">
         <v>25</v>
@@ -9726,7 +9778,7 @@
         <v>1.1304347826086958</v>
       </c>
       <c r="E150" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F150" s="0">
         <v>26</v>
@@ -9746,7 +9798,7 @@
         <v>0.73333333333333328</v>
       </c>
       <c r="E151" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F151" s="0">
         <v>27</v>
@@ -9766,7 +9818,7 @@
         <v>0.70370370370370372</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F152" s="0">
         <v>28</v>
@@ -9786,7 +9838,7 @@
         <v>0.65000000000000002</v>
       </c>
       <c r="E153" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F153" s="0">
         <v>29</v>
@@ -9806,7 +9858,7 @@
         <v>0.45945945945945948</v>
       </c>
       <c r="E154" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F154" s="0">
         <v>30</v>
@@ -9826,7 +9878,7 @@
         <v>0.2950819672131148</v>
       </c>
       <c r="E155" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F155" s="0">
         <v>31</v>
@@ -9846,7 +9898,7 @@
         <v>1.0803571428571428</v>
       </c>
       <c r="E156" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F156" s="0">
         <v>32</v>
@@ -9866,7 +9918,7 @@
         <v>0.35294117647058826</v>
       </c>
       <c r="E157" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F157" s="0">
         <v>33</v>
@@ -9886,7 +9938,7 @@
         <v>0.79411764705882359</v>
       </c>
       <c r="E158" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F158" s="0">
         <v>34</v>
@@ -9906,7 +9958,7 @@
         <v>0.84374999999999989</v>
       </c>
       <c r="E159" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F159" s="0">
         <v>35</v>
@@ -9926,7 +9978,7 @@
         <v>1.173913043478261</v>
       </c>
       <c r="E160" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F160" s="0">
         <v>36</v>
@@ -9946,7 +9998,7 @@
         <v>0.81999999999999995</v>
       </c>
       <c r="E161" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F161" s="0">
         <v>37</v>
@@ -9966,7 +10018,7 @@
         <v>0.64516129032258074</v>
       </c>
       <c r="E162" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F162" s="0">
         <v>38</v>
@@ -9986,7 +10038,7 @@
         <v>0.71794871794871784</v>
       </c>
       <c r="E163" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F163" s="0">
         <v>39</v>
@@ -10006,7 +10058,7 @@
         <v>1.0373134328358207</v>
       </c>
       <c r="E164" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F164" s="0">
         <v>40</v>
@@ -10026,7 +10078,7 @@
         <v>1.0305343511450382</v>
       </c>
       <c r="E165" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F165" s="0">
         <v>41</v>
@@ -10046,7 +10098,7 @@
         <v>0.85245901639344268</v>
       </c>
       <c r="E166" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F166" s="0">
         <v>42</v>
@@ -10066,7 +10118,7 @@
         <v>0.81944444444444442</v>
       </c>
       <c r="E167" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F167" s="0">
         <v>43</v>
@@ -10086,7 +10138,7 @@
         <v>0.92771084337349408</v>
       </c>
       <c r="E168" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F168" s="0">
         <v>44</v>
@@ -10106,7 +10158,7 @@
         <v>0.95061728395061729</v>
       </c>
       <c r="E169" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F169" s="0">
         <v>45</v>
@@ -10126,7 +10178,7 @@
         <v>0.93684210526315792</v>
       </c>
       <c r="E170" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F170" s="0">
         <v>46</v>
@@ -10146,7 +10198,7 @@
         <v>0.97402597402597391</v>
       </c>
       <c r="E171" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F171" s="0">
         <v>47</v>
@@ -10166,7 +10218,7 @@
         <v>0.77551020408163263</v>
       </c>
       <c r="E172" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F172" s="0">
         <v>48</v>
@@ -10186,7 +10238,7 @@
         <v>0.98000000000000009</v>
       </c>
       <c r="E173" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F173" s="0">
         <v>49</v>
@@ -10206,7 +10258,7 @@
         <v>0.81651376146789001</v>
       </c>
       <c r="E174" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F174" s="0">
         <v>50</v>
@@ -10226,7 +10278,7 @@
         <v>0.91999999999999993</v>
       </c>
       <c r="E175" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F175" s="0">
         <v>51</v>
@@ -10246,7 +10298,7 @@
         <v>0.9316546762589929</v>
       </c>
       <c r="E176" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F176" s="0">
         <v>52</v>
@@ -10266,7 +10318,7 @@
         <v>0.67346938775510201</v>
       </c>
       <c r="E177" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F177" s="0">
         <v>53</v>
@@ -10286,7 +10338,7 @@
         <v>0.43243243243243251</v>
       </c>
       <c r="E178" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F178" s="0">
         <v>54</v>
@@ -10306,7 +10358,7 @@
         <v>0.98333333333333328</v>
       </c>
       <c r="E179" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F179" s="0">
         <v>55</v>
@@ -10326,7 +10378,7 @@
         <v>0.96634615384615385</v>
       </c>
       <c r="E180" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F180" s="0">
         <v>56</v>
@@ -10346,7 +10398,7 @@
         <v>0.69696969696969691</v>
       </c>
       <c r="E181" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F181" s="0">
         <v>57</v>
@@ -10366,7 +10418,7 @@
         <v>0.73809523809523814</v>
       </c>
       <c r="E182" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F182" s="0">
         <v>58</v>
@@ -10386,7 +10438,7 @@
         <v>1.1808510638297871</v>
       </c>
       <c r="E183" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F183" s="0">
         <v>59</v>
@@ -10406,7 +10458,7 @@
         <v>1.1935483870967742</v>
       </c>
       <c r="E184" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F184" s="0">
         <v>60</v>
@@ -10426,7 +10478,7 @@
         <v>1.0138888888888888</v>
       </c>
       <c r="E185" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F185" s="0">
         <v>61</v>
@@ -10446,7 +10498,7 @@
         <v>0.6914893617021276</v>
       </c>
       <c r="E186" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F186" s="0">
         <v>62</v>
@@ -10466,7 +10518,7 @@
         <v>0.84999999999999998</v>
       </c>
       <c r="E187" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F187" s="0">
         <v>63</v>
@@ -10486,7 +10538,7 @@
         <v>0.79518072289156627</v>
       </c>
       <c r="E188" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F188" s="0">
         <v>64</v>
@@ -10506,7 +10558,7 @@
         <v>0.58823529411764708</v>
       </c>
       <c r="E189" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F189" s="0">
         <v>65</v>
@@ -10526,7 +10578,7 @@
         <v>0.76190476190476208</v>
       </c>
       <c r="E190" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F190" s="0">
         <v>66</v>
@@ -10546,7 +10598,7 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="E191" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F191" s="0">
         <v>67</v>
@@ -10566,7 +10618,7 @@
         <v>0.83870967741935487</v>
       </c>
       <c r="E192" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F192" s="0">
         <v>68</v>
@@ -10586,7 +10638,7 @@
         <v>0.40157480314960625</v>
       </c>
       <c r="E193" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F193" s="0">
         <v>69</v>
@@ -10606,7 +10658,7 @@
         <v>0.84999999999999987</v>
       </c>
       <c r="E194" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F194" s="0">
         <v>70</v>
@@ -10626,7 +10678,7 @@
         <v>1</v>
       </c>
       <c r="E195" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F195" s="0">
         <v>71</v>
@@ -10646,7 +10698,7 @@
         <v>0.84615384615384615</v>
       </c>
       <c r="E196" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F196" s="0">
         <v>72</v>
@@ -10666,7 +10718,7 @@
         <v>0.72897196261682251</v>
       </c>
       <c r="E197" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F197" s="0">
         <v>73</v>
@@ -10686,7 +10738,7 @@
         <v>0.70491803278688536</v>
       </c>
       <c r="E198" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F198" s="0">
         <v>74</v>
@@ -10706,7 +10758,7 @@
         <v>0.71428571428571441</v>
       </c>
       <c r="E199" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F199" s="0">
         <v>75</v>
@@ -10726,7 +10778,7 @@
         <v>0.54761904761904767</v>
       </c>
       <c r="E200" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F200" s="0">
         <v>76</v>
@@ -10746,7 +10798,7 @@
         <v>0.61666666666666659</v>
       </c>
       <c r="E201" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F201" s="0">
         <v>77</v>
@@ -10766,7 +10818,7 @@
         <v>0.92307692307692291</v>
       </c>
       <c r="E202" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F202" s="0">
         <v>78</v>
@@ -10786,7 +10838,7 @@
         <v>0.51063829787234039</v>
       </c>
       <c r="E203" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F203" s="0">
         <v>79</v>
@@ -10806,7 +10858,7 @@
         <v>0.61643835616438358</v>
       </c>
       <c r="E204" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F204" s="0">
         <v>80</v>
@@ -10826,7 +10878,7 @@
         <v>0.48888888888888887</v>
       </c>
       <c r="E205" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F205" s="0">
         <v>81</v>
@@ -10846,7 +10898,7 @@
         <v>0.77777777777777768</v>
       </c>
       <c r="E206" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F206" s="0">
         <v>82</v>
@@ -10866,7 +10918,7 @@
         <v>0.76190476190476208</v>
       </c>
       <c r="E207" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F207" s="0">
         <v>83</v>
@@ -10886,7 +10938,7 @@
         <v>0.49180327868852469</v>
       </c>
       <c r="E208" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F208" s="0">
         <v>84</v>
@@ -10906,7 +10958,7 @@
         <v>0.82198952879581144</v>
       </c>
       <c r="E209" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F209" s="0">
         <v>85</v>
@@ -10926,7 +10978,7 @@
         <v>0.93617021276595735</v>
       </c>
       <c r="E210" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F210" s="0">
         <v>86</v>
@@ -10946,7 +10998,7 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="E211" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F211" s="0">
         <v>87</v>
@@ -10966,7 +11018,7 @@
         <v>0.38095238095238104</v>
       </c>
       <c r="E212" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F212" s="0">
         <v>88</v>
@@ -10986,7 +11038,7 @@
         <v>0.68000000000000005</v>
       </c>
       <c r="E213" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F213" s="0">
         <v>89</v>
@@ -11006,7 +11058,7 @@
         <v>0.47727272727272724</v>
       </c>
       <c r="E214" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F214" s="0">
         <v>90</v>
@@ -11026,7 +11078,7 @@
         <v>0.7831325301204819</v>
       </c>
       <c r="E215" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F215" s="0">
         <v>91</v>
@@ -11046,7 +11098,7 @@
         <v>0.52054794520547953</v>
       </c>
       <c r="E216" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F216" s="0">
         <v>92</v>
@@ -11066,7 +11118,7 @@
         <v>0.45121951219512191</v>
       </c>
       <c r="E217" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F217" s="0">
         <v>93</v>
@@ -11086,7 +11138,7 @@
         <v>0.75000000000000011</v>
       </c>
       <c r="E218" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F218" s="0">
         <v>94</v>
@@ -11106,7 +11158,7 @@
         <v>0.76842105263157889</v>
       </c>
       <c r="E219" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F219" s="0">
         <v>95</v>
@@ -11126,7 +11178,7 @@
         <v>0.50793650793650802</v>
       </c>
       <c r="E220" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F220" s="0">
         <v>96</v>
@@ -11146,7 +11198,7 @@
         <v>0.87499999999999989</v>
       </c>
       <c r="E221" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F221" s="0">
         <v>97</v>
@@ -11166,7 +11218,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E222" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F222" s="0">
         <v>98</v>
@@ -11186,7 +11238,7 @@
         <v>0.70967741935483863</v>
       </c>
       <c r="E223" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F223" s="0">
         <v>99</v>
@@ -11206,7 +11258,7 @@
         <v>1.3157894736842104</v>
       </c>
       <c r="E224" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F224" s="0">
         <v>100</v>
@@ -11226,7 +11278,7 @@
         <v>1.2222222222222221</v>
       </c>
       <c r="E225" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F225" s="0">
         <v>101</v>
@@ -11246,7 +11298,7 @@
         <v>1.0597014925373134</v>
       </c>
       <c r="E226" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F226" s="0">
         <v>102</v>
@@ -11266,7 +11318,7 @@
         <v>1.0121951219512195</v>
       </c>
       <c r="E227" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F227" s="0">
         <v>103</v>
@@ -11286,7 +11338,7 @@
         <v>0.71999999999999997</v>
       </c>
       <c r="E228" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F228" s="0">
         <v>104</v>
@@ -11306,7 +11358,7 @@
         <v>0.65384615384615374</v>
       </c>
       <c r="E229" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F229" s="0">
         <v>105</v>
@@ -11326,7 +11378,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E230" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F230" s="0">
         <v>106</v>
@@ -11346,7 +11398,7 @@
         <v>0.43478260869565222</v>
       </c>
       <c r="E231" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F231" s="0">
         <v>107</v>
@@ -11366,7 +11418,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E232" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F232" s="0">
         <v>108</v>
@@ -11386,7 +11438,7 @@
         <v>0.79310344827586199</v>
       </c>
       <c r="E233" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F233" s="0">
         <v>109</v>
@@ -11406,7 +11458,7 @@
         <v>0.65384615384615385</v>
       </c>
       <c r="E234" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F234" s="0">
         <v>110</v>
@@ -11426,7 +11478,7 @@
         <v>0.77358490566037741</v>
       </c>
       <c r="E235" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F235" s="0">
         <v>111</v>
@@ -11446,7 +11498,7 @@
         <v>0.79746835443037989</v>
       </c>
       <c r="E236" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F236" s="0">
         <v>112</v>
@@ -11466,7 +11518,7 @@
         <v>0.62962962962962965</v>
       </c>
       <c r="E237" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F237" s="0">
         <v>113</v>
@@ -11486,7 +11538,7 @@
         <v>0.61904761904761907</v>
       </c>
       <c r="E238" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F238" s="0">
         <v>114</v>
@@ -11506,7 +11558,7 @@
         <v>0.73333333333333328</v>
       </c>
       <c r="E239" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F239" s="0">
         <v>115</v>
@@ -11526,7 +11578,7 @@
         <v>0.7661290322580645</v>
       </c>
       <c r="E240" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F240" s="0">
         <v>116</v>
@@ -11546,7 +11598,7 @@
         <v>0.676056338028169</v>
       </c>
       <c r="E241" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F241" s="0">
         <v>117</v>
@@ -11566,7 +11618,7 @@
         <v>0.80303030303030298</v>
       </c>
       <c r="E242" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F242" s="0">
         <v>118</v>
@@ -11586,7 +11638,7 @@
         <v>1.0222222222222221</v>
       </c>
       <c r="E243" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F243" s="0">
         <v>119</v>
@@ -11606,7 +11658,7 @@
         <v>0.7831325301204819</v>
       </c>
       <c r="E244" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F244" s="0">
         <v>120</v>
@@ -11626,7 +11678,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E245" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F245" s="0">
         <v>121</v>
@@ -11646,7 +11698,7 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="E246" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F246" s="0">
         <v>122</v>
@@ -11666,7 +11718,7 @@
         <v>0.34374999999999994</v>
       </c>
       <c r="E247" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F247" s="0">
         <v>123</v>

</xml_diff>